<commit_message>
last plots for LaP presentation
</commit_message>
<xml_diff>
--- a/Model_analysis/Sensitivity-analysis/v1.1_November2022/Parameter_table.xlsx
+++ b/Model_analysis/Sensitivity-analysis/v1.1_November2022/Parameter_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Documentos\github\BLT_IBM-Model\Model_analysis\Sensitivity-analysis\v1.1_November2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E4C81A-9D08-45A1-8F29-E1FF58B2E153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76499D46-FFA6-4909-BA9E-C19168535150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -751,12 +751,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -824,6 +818,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1182,7 +1182,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A8" sqref="A8:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1198,20 +1198,20 @@
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="13" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="14"/>
+      <c r="I1" s="43"/>
       <c r="J1" s="2" t="s">
         <v>33</v>
       </c>
@@ -1249,7 +1249,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="5">
@@ -1281,7 +1281,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="32" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5">
@@ -1313,7 +1313,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="32" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="5">
@@ -1345,70 +1345,70 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="27">
         <v>13.871047350989899</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="28">
         <v>12.9337858396692</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="28">
         <v>12.1373560652533</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="28">
         <v>14.060271552203499</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="27">
         <v>21.034303941083</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="28">
         <v>16.949538942060599</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="28">
         <v>8.3843268713118597</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="28">
         <v>7.5107447858649996</v>
       </c>
-      <c r="J6" s="30">
+      <c r="J6" s="28">
         <v>30.887319222552001</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="23">
         <v>25.3008138996125</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="24">
         <v>25.199517954068899</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="24">
         <v>25.441482821043198</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="24">
         <v>23.426252956065799</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="23">
         <v>35.971099115842897</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="24">
         <v>32.374746763730997</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="24">
         <v>17.489357303595</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="24">
         <v>17.935822633893899</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="24">
         <v>39.306009261536097</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1440,39 +1440,39 @@
         <v>9.7747038491729494</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="17">
         <v>15.7471396125556</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="18">
         <v>17.296123683991201</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="18">
         <v>19.4057102365906</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="18">
         <v>18.0080855378405</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="17">
         <v>26.591422085730599</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="18">
         <v>21.302313807533199</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="18">
         <v>6.5629028115306403</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="18">
         <v>7.0856773741182097</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="18">
         <v>13.2060760646049</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>66.814664626610394</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>70.769334990690496</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>73.804005910665595</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1600,39 +1600,39 @@
         <v>97.325663437133997</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="14">
         <v>114.986316542167</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="15">
         <v>121.11955311267501</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="15">
         <v>124.72075714619901</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="15">
         <v>138.62649541025601</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="14">
         <v>122.665615422215</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G14" s="15">
         <v>158.88861745993401</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="15">
         <v>101.766907272395</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I14" s="15">
         <v>96.948125437174994</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J14" s="15">
         <v>74.845622849586903</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1665,162 +1665,162 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="23">
         <v>77.224154337015705</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="24">
         <v>75.660787787241503</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="24">
         <v>78.994701436733493</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="24">
         <v>68.978090978214794</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="23">
         <v>62.996745356243601</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G16" s="24">
         <v>89.728795039418003</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="24">
         <v>51.203918456164601</v>
       </c>
-      <c r="I16" s="26">
+      <c r="I16" s="24">
         <v>55.919073085186596</v>
       </c>
-      <c r="J16" s="26">
+      <c r="J16" s="24">
         <v>43.015297395262998</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="25">
         <v>59.534454595372999</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="26">
         <v>72.7531475671815</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="26">
         <v>75.625732874087205</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="26">
         <v>67.861888611224401</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="25">
         <v>58.758088486745898</v>
       </c>
-      <c r="G17" s="28">
+      <c r="G17" s="26">
         <v>68.994893947621193</v>
       </c>
-      <c r="H17" s="28">
+      <c r="H17" s="26">
         <v>47.528428193934602</v>
       </c>
-      <c r="I17" s="28">
+      <c r="I17" s="26">
         <v>63.6138500423639</v>
       </c>
-      <c r="J17" s="28">
+      <c r="J17" s="26">
         <v>17.853706346809499</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="36">
+      <c r="B18" s="34">
         <v>0.69787120191031304</v>
       </c>
-      <c r="C18" s="37">
+      <c r="C18" s="35">
         <v>0.536646016086892</v>
       </c>
-      <c r="D18" s="37">
+      <c r="D18" s="35">
         <v>0.47385577994325401</v>
       </c>
-      <c r="E18" s="37">
+      <c r="E18" s="35">
         <v>0.362358870393786</v>
       </c>
-      <c r="F18" s="36">
+      <c r="F18" s="34">
         <v>0.61318570881173595</v>
       </c>
-      <c r="G18" s="37">
+      <c r="G18" s="35">
         <v>0.59293823763793896</v>
       </c>
-      <c r="H18" s="37">
+      <c r="H18" s="35">
         <v>0.206769100095304</v>
       </c>
-      <c r="I18" s="37">
+      <c r="I18" s="35">
         <v>0.31034221109340598</v>
       </c>
-      <c r="J18" s="37">
+      <c r="J18" s="35">
         <v>0.21311777308358301</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="40">
+      <c r="B19" s="38">
         <v>19</v>
       </c>
-      <c r="C19" s="41">
+      <c r="C19" s="39">
         <v>13</v>
       </c>
-      <c r="D19" s="41">
+      <c r="D19" s="39">
         <v>18</v>
       </c>
-      <c r="E19" s="41">
+      <c r="E19" s="39">
         <v>17</v>
       </c>
-      <c r="F19" s="40">
+      <c r="F19" s="38">
         <v>16.600000000000001</v>
       </c>
-      <c r="G19" s="42">
+      <c r="G19" s="40">
         <v>16</v>
       </c>
-      <c r="H19" s="41">
+      <c r="H19" s="39">
         <v>21</v>
       </c>
-      <c r="I19" s="41">
+      <c r="I19" s="39">
         <v>26</v>
       </c>
-      <c r="J19" s="41">
+      <c r="J19" s="39">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="40">
+      <c r="B20" s="38">
         <v>9</v>
       </c>
-      <c r="C20" s="41">
+      <c r="C20" s="39">
         <v>6</v>
       </c>
-      <c r="D20" s="41">
+      <c r="D20" s="39">
         <v>10</v>
       </c>
-      <c r="E20" s="41">
+      <c r="E20" s="39">
         <v>11</v>
       </c>
-      <c r="F20" s="40">
+      <c r="F20" s="38">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G20" s="42">
+      <c r="G20" s="40">
         <v>12</v>
       </c>
-      <c r="H20" s="41">
+      <c r="H20" s="39">
         <v>9</v>
       </c>
-      <c r="I20" s="41">
+      <c r="I20" s="39">
         <v>9</v>
       </c>
-      <c r="J20" s="41">
+      <c r="J20" s="39">
         <v>7</v>
       </c>
     </row>
@@ -1889,66 +1889,66 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="21">
+      <c r="B23" s="19">
         <v>77</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="20">
         <v>86</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="20">
         <v>43</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="20">
         <v>28</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F23" s="19">
         <v>43</v>
       </c>
-      <c r="G23" s="22">
+      <c r="G23" s="20">
         <v>61</v>
       </c>
-      <c r="H23" s="22">
+      <c r="H23" s="20">
         <v>46</v>
       </c>
-      <c r="I23" s="22">
+      <c r="I23" s="20">
         <v>27</v>
       </c>
-      <c r="J23" s="22">
+      <c r="J23" s="20">
         <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="21">
         <v>7</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="22">
         <v>8</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="22">
         <v>5</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="22">
         <v>1</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="21">
         <v>2</v>
       </c>
-      <c r="G24" s="24">
+      <c r="G24" s="22">
         <v>6</v>
       </c>
-      <c r="H24" s="24">
+      <c r="H24" s="22">
         <v>7</v>
       </c>
-      <c r="I24" s="24">
+      <c r="I24" s="22">
         <v>3</v>
       </c>
-      <c r="J24" s="24">
+      <c r="J24" s="22">
         <v>7</v>
       </c>
     </row>

</xml_diff>